<commit_message>
Power BI Telework Dashboard Template
</commit_message>
<xml_diff>
--- a/Template/Employees Telework Details.xlsx
+++ b/Template/Employees Telework Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KWhite\Clients\ETS\TeleworkDashboard\PowerBI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75596A3A-1A8C-4D1E-A935-C8FED9BEB932}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A1DC5A-0991-4E5A-A2C9-C0EEA780EC72}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="1125" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees Telework Details" sheetId="4" r:id="rId1"/>
@@ -148,10 +148,6 @@
     <t>3. This sample dataset contains the data for multiple weeks (9/14, 9/21 and 9/28).</t>
   </si>
   <si>
-    <t>Note the date the report was ran.
-This should be generated on a Monday projecting the week's data. For example, if the report date is 9/14, then this report covers 9/14 through 9/20.</t>
-  </si>
-  <si>
     <t>2. If alternate work week is not provided, standard (5-8-40) will be assumed.</t>
   </si>
   <si>
@@ -159,6 +155,9 @@
 Standard
 FT_AWWS 9/8/80
 FT_AWWS 4/10/40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date that the report was run.  This report should be run weekly and submitted to DGS every Monday by 5pm.  </t>
   </si>
 </sst>
 </file>
@@ -662,7 +661,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -686,9 +685,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -791,8 +787,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB855020-9AC8-4630-89A0-A8FFA8ADF89B}" name="Table1" displayName="Table1" ref="A7:D16" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A7:D16" xr:uid="{6269FD2E-EF22-4C09-A5AB-0B07FA219221}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB855020-9AC8-4630-89A0-A8FFA8ADF89B}" name="Table1" displayName="Table1" ref="A7:D17" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A7:D17" xr:uid="{6269FD2E-EF22-4C09-A5AB-0B07FA219221}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0AE1842A-08CC-4934-8EA5-015CE802D4F4}" name="Field Name" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{06789D9D-1099-46FF-B441-743DAF457832}" name="Definition" dataDxfId="2"/>
@@ -69818,10 +69814,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7CAFEA6-1537-45A9-8E97-2A0C21FE1C87}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -69858,7 +69854,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
@@ -69954,9 +69950,9 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -70002,12 +69998,12 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>34</v>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>12</v>
@@ -70015,6 +70011,12 @@
       <c r="D16" s="7">
         <v>44088</v>
       </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A10:C10">

</xml_diff>